<commit_message>
BD ok, Budget ok, mail ok --> menu deroulant
</commit_message>
<xml_diff>
--- a/time/gantt.xlsx
+++ b/time/gantt.xlsx
@@ -1,31 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariejessica\Desktop\Projet Individuel\INFOB318-bump\time\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="15000" windowHeight="8475"/>
   </bookViews>
   <sheets>
     <sheet name="effort" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
-  <si>
-    <t>Analyse</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>Rencontre client</t>
-  </si>
-  <si>
-    <t>Correction</t>
-  </si>
-  <si>
-    <t>Conception</t>
   </si>
   <si>
     <t>correction</t>
@@ -62,6 +58,33 @@
   </si>
   <si>
     <t>Projet:</t>
+  </si>
+  <si>
+    <t>Analyse du sujet</t>
+  </si>
+  <si>
+    <t>familiarisation du matériel</t>
+  </si>
+  <si>
+    <t>BUMP</t>
+  </si>
+  <si>
+    <t>2015-2016</t>
+  </si>
+  <si>
+    <t>marie</t>
+  </si>
+  <si>
+    <t>ntumb an mwinkeu</t>
+  </si>
+  <si>
+    <t>conception</t>
+  </si>
+  <si>
+    <t>comprehension partie antérieure</t>
+  </si>
+  <si>
+    <t>modelisation</t>
   </si>
 </sst>
 </file>
@@ -148,7 +171,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -417,6 +440,15 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -428,7 +460,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1"/>
@@ -469,10 +501,11 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="5" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="5" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20 % - Accent1" xfId="1" builtinId="30"/>
@@ -487,6 +520,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -535,7 +571,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -570,7 +606,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -779,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y44"/>
+  <dimension ref="A1:Y47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,93 +834,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+    </row>
+    <row r="2" spans="1:25" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="1:25" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+    </row>
+    <row r="4" spans="1:25" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-    </row>
-    <row r="2" spans="1:25" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-    </row>
-    <row r="3" spans="1:25" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-    </row>
-    <row r="4" spans="1:25" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="25" t="s">
+      <c r="B4" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6" s="22">
-        <f>SUM(C9:C34)</f>
-        <v>13</v>
+        <f t="shared" ref="C6:Y6" si="0">SUM(C9:C37)</f>
+        <v>0</v>
       </c>
       <c r="D6" s="23">
-        <f t="shared" ref="D6:Y6" si="0">SUM(D9:D34)</f>
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="E6" s="23">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F6" s="23">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L6" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M6" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="5">
         <f t="shared" si="0"/>
@@ -937,10 +981,10 @@
     </row>
     <row r="7" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1">
         <v>42282</v>
@@ -1036,21 +1080,18 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="18">
-        <f>SUM(C8:Y8)</f>
-        <v>12</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B8" s="18"/>
       <c r="C8" s="19"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="12">
-        <v>12</v>
-      </c>
+      <c r="G8" s="12"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="I8" s="12">
+        <v>14</v>
+      </c>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
@@ -1070,16 +1111,13 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="14">
         <v>1</v>
       </c>
-      <c r="B9" s="9">
-        <f>SUM(C9:Y9)</f>
-        <v>1</v>
-      </c>
-      <c r="C9" s="20">
-        <v>1</v>
-      </c>
-      <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
@@ -1104,19 +1142,16 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="9">
-        <f t="shared" ref="B10:B27" si="11">SUM(C10:Y10)</f>
-        <v>24</v>
-      </c>
-      <c r="C10" s="20">
-        <v>12</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="14">
-        <v>12</v>
-      </c>
-      <c r="E10" s="14"/>
+        <v>5</v>
+      </c>
+      <c r="E10" s="14">
+        <v>5</v>
+      </c>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -1140,16 +1175,13 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="9">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B11" s="9"/>
       <c r="C11" s="20"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
@@ -1174,19 +1206,18 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="9">
-        <f t="shared" si="11"/>
-        <v>3</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B12" s="9"/>
       <c r="C12" s="20"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="G12" s="14">
+        <v>7</v>
+      </c>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
@@ -1207,19 +1238,16 @@
       <c r="Y12" s="15"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="9">
-        <f t="shared" si="11"/>
-        <v>7</v>
-      </c>
+      <c r="A13" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="9"/>
       <c r="C13" s="20"/>
       <c r="D13" s="14"/>
-      <c r="E13" s="14">
-        <v>7</v>
-      </c>
-      <c r="F13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14">
+        <v>1</v>
+      </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
@@ -1244,15 +1272,12 @@
       <c r="A14" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="9">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
+      <c r="B14" s="9"/>
       <c r="C14" s="20"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -1276,19 +1301,18 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="9">
-        <f t="shared" si="11"/>
-        <v>3</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B15" s="9"/>
       <c r="C15" s="20"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14">
-        <v>3</v>
-      </c>
-      <c r="G15" s="14"/>
+        <v>5</v>
+      </c>
+      <c r="G15" s="14">
+        <v>10</v>
+      </c>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
@@ -1310,26 +1334,29 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="9">
-        <f t="shared" si="11"/>
-        <v>14</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B16" s="9"/>
       <c r="C16" s="20"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
-      <c r="F16" s="14">
+      <c r="F16" s="14"/>
+      <c r="G16" s="14">
+        <v>12</v>
+      </c>
+      <c r="H16" s="14">
+        <v>12</v>
+      </c>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14">
+        <v>10</v>
+      </c>
+      <c r="K16" s="14">
         <v>7</v>
       </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14">
+      <c r="L16" s="14">
         <v>7</v>
       </c>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
       <c r="M16" s="14"/>
       <c r="N16" s="14"/>
       <c r="O16" s="14"/>
@@ -1346,25 +1373,24 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="9">
-        <f t="shared" si="11"/>
-        <v>3</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B17" s="9"/>
       <c r="C17" s="20"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
-      <c r="I17" s="14">
-        <v>3</v>
-      </c>
-      <c r="J17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14">
+        <v>1</v>
+      </c>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
+      <c r="M17" s="14">
+        <v>1</v>
+      </c>
       <c r="N17" s="14"/>
       <c r="O17" s="14"/>
       <c r="P17" s="14"/>
@@ -1380,21 +1406,16 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="9">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B18" s="9"/>
       <c r="C18" s="20"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
-      <c r="I18" s="14">
-        <v>1</v>
-      </c>
+      <c r="I18" s="14"/>
       <c r="J18" s="14"/>
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
@@ -1414,12 +1435,9 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B19" s="9"/>
       <c r="C19" s="20"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
@@ -1446,12 +1464,9 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B20" s="9"/>
       <c r="C20" s="20"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
@@ -1478,12 +1493,9 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B21" s="9"/>
       <c r="C21" s="20"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
@@ -1510,12 +1522,9 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B22" s="9"/>
       <c r="C22" s="20"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
@@ -1542,12 +1551,9 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B23" s="9"/>
       <c r="C23" s="20"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
@@ -1574,12 +1580,9 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B24" s="9"/>
       <c r="C24" s="20"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
@@ -1606,12 +1609,9 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B25" s="9"/>
       <c r="C25" s="20"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
@@ -1638,12 +1638,9 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B26" s="9"/>
       <c r="C26" s="20"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
@@ -1669,11 +1666,10 @@
       <c r="Y26" s="15"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
+      <c r="A27" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="9"/>
       <c r="C27" s="20"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
@@ -1699,11 +1695,10 @@
       <c r="Y27" s="15"/>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9">
-        <f t="shared" ref="B28:B38" si="12">SUM(C28:Y28)</f>
-        <v>0</v>
-      </c>
+      <c r="A28" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="9"/>
       <c r="C28" s="20"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
@@ -1730,10 +1725,7 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
-      <c r="B29" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
+      <c r="B29" s="9"/>
       <c r="C29" s="20"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
@@ -1760,10 +1752,7 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
-      <c r="B30" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
+      <c r="B30" s="9"/>
       <c r="C30" s="20"/>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
@@ -1790,10 +1779,7 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
-      <c r="B31" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
+      <c r="B31" s="9"/>
       <c r="C31" s="20"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
@@ -1820,10 +1806,7 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
-      <c r="B32" s="9">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
+      <c r="B32" s="9"/>
       <c r="C32" s="20"/>
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
@@ -1848,12 +1831,9 @@
       <c r="X32" s="14"/>
       <c r="Y32" s="15"/>
     </row>
-    <row r="33" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
       <c r="C33" s="20"/>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
@@ -1879,11 +1859,9 @@
       <c r="Y33" s="15"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="A34" s="9"/>
       <c r="B34" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="B34:B41" si="11">SUM(C34:Y34)</f>
         <v>0</v>
       </c>
       <c r="C34" s="20"/>
@@ -1910,12 +1888,10 @@
       <c r="X34" s="14"/>
       <c r="Y34" s="15"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>7</v>
-      </c>
+    <row r="35" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="10"/>
       <c r="B35" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="C35" s="20"/>
@@ -1942,12 +1918,12 @@
       <c r="X35" s="14"/>
       <c r="Y35" s="15"/>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="9">
-        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="B36" s="10">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="C36" s="20"/>
@@ -1976,10 +1952,10 @@
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B37" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="C37" s="20"/>
@@ -2007,9 +1983,11 @@
       <c r="Y37" s="15"/>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
+      <c r="A38" s="9" t="s">
+        <v>4</v>
+      </c>
       <c r="B38" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="C38" s="20"/>
@@ -2037,9 +2015,11 @@
       <c r="Y38" s="15"/>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
+      <c r="A39" s="9" t="s">
+        <v>4</v>
+      </c>
       <c r="B39" s="9">
-        <f t="shared" ref="B39:B44" si="13">SUM(C39:Y39)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="C39" s="20"/>
@@ -2069,7 +2049,7 @@
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="B40" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="C40" s="20"/>
@@ -2099,7 +2079,7 @@
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="B41" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="C41" s="20"/>
@@ -2129,7 +2109,7 @@
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="B42" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="B42:B47" si="12">SUM(C42:Y42)</f>
         <v>0</v>
       </c>
       <c r="C42" s="20"/>
@@ -2159,7 +2139,7 @@
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
       <c r="B43" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="C43" s="20"/>
@@ -2186,35 +2166,124 @@
       <c r="X43" s="14"/>
       <c r="Y43" s="15"/>
     </row>
-    <row r="44" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="C44" s="21"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
-      <c r="I44" s="16"/>
-      <c r="J44" s="16"/>
-      <c r="K44" s="16"/>
-      <c r="L44" s="16"/>
-      <c r="M44" s="16"/>
-      <c r="N44" s="16"/>
-      <c r="O44" s="16"/>
-      <c r="P44" s="16"/>
-      <c r="Q44" s="16"/>
-      <c r="R44" s="16"/>
-      <c r="S44" s="16"/>
-      <c r="T44" s="16"/>
-      <c r="U44" s="16"/>
-      <c r="V44" s="16"/>
-      <c r="W44" s="16"/>
-      <c r="X44" s="16"/>
-      <c r="Y44" s="17"/>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A44" s="9"/>
+      <c r="B44" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="C44" s="20"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
+      <c r="T44" s="14"/>
+      <c r="U44" s="14"/>
+      <c r="V44" s="14"/>
+      <c r="W44" s="14"/>
+      <c r="X44" s="14"/>
+      <c r="Y44" s="15"/>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="C45" s="20"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+      <c r="M45" s="14"/>
+      <c r="N45" s="14"/>
+      <c r="O45" s="14"/>
+      <c r="P45" s="14"/>
+      <c r="Q45" s="14"/>
+      <c r="R45" s="14"/>
+      <c r="S45" s="14"/>
+      <c r="T45" s="14"/>
+      <c r="U45" s="14"/>
+      <c r="V45" s="14"/>
+      <c r="W45" s="14"/>
+      <c r="X45" s="14"/>
+      <c r="Y45" s="15"/>
+    </row>
+    <row r="46" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="10"/>
+      <c r="B46" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="C46" s="20"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14"/>
+      <c r="M46" s="14"/>
+      <c r="N46" s="14"/>
+      <c r="O46" s="14"/>
+      <c r="P46" s="14"/>
+      <c r="Q46" s="14"/>
+      <c r="R46" s="14"/>
+      <c r="S46" s="14"/>
+      <c r="T46" s="14"/>
+      <c r="U46" s="14"/>
+      <c r="V46" s="14"/>
+      <c r="W46" s="14"/>
+      <c r="X46" s="14"/>
+      <c r="Y46" s="15"/>
+    </row>
+    <row r="47" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="10">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="C47" s="21"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
+      <c r="M47" s="16"/>
+      <c r="N47" s="16"/>
+      <c r="O47" s="16"/>
+      <c r="P47" s="16"/>
+      <c r="Q47" s="16"/>
+      <c r="R47" s="16"/>
+      <c r="S47" s="16"/>
+      <c r="T47" s="16"/>
+      <c r="U47" s="16"/>
+      <c r="V47" s="16"/>
+      <c r="W47" s="16"/>
+      <c r="X47" s="16"/>
+      <c r="Y47" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2223,42 +2292,8 @@
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:F4"/>
   </mergeCells>
-  <conditionalFormatting sqref="B9:B27">
-    <cfRule type="dataBar" priority="26">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4522925B-D263-4740-830B-036B98A7E6A9}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9:O16 C19:O27 C17:G18 I17:O18">
+  <conditionalFormatting sqref="C22:O30 C9:O19 C20:G21 I20:O21">
     <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8:P8 P9:P27">
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q8:Y27">
-    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2281,7 +2316,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B28">
+  <conditionalFormatting sqref="B31">
     <cfRule type="dataBar" priority="19">
       <dataBar>
         <cfvo type="min"/>
@@ -2295,7 +2330,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:O28">
+  <conditionalFormatting sqref="C31:O31">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -2305,7 +2340,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P28">
+  <conditionalFormatting sqref="P31">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -2315,7 +2350,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q28:Y28">
+  <conditionalFormatting sqref="Q31:Y31">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -2325,7 +2360,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29:B33">
+  <conditionalFormatting sqref="B32:B36">
     <cfRule type="dataBar" priority="15">
       <dataBar>
         <cfvo type="min"/>
@@ -2339,7 +2374,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:O33">
+  <conditionalFormatting sqref="C32:O36">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -2349,7 +2384,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P29:P33">
+  <conditionalFormatting sqref="P32:P36">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -2359,7 +2394,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q29:Y33">
+  <conditionalFormatting sqref="Q32:Y36">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -2369,7 +2404,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B34:B38">
+  <conditionalFormatting sqref="B37:B41">
     <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="min"/>
@@ -2383,7 +2418,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34:O38">
+  <conditionalFormatting sqref="C37:O41">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -2393,7 +2428,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P34:P38">
+  <conditionalFormatting sqref="P37:P41">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -2403,7 +2438,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q34:Y38">
+  <conditionalFormatting sqref="Q37:Y41">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -2413,7 +2448,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B39">
+  <conditionalFormatting sqref="B42">
     <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
@@ -2427,7 +2462,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C39:O39">
+  <conditionalFormatting sqref="C42:O42">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -2437,7 +2472,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P39">
+  <conditionalFormatting sqref="P42">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2447,7 +2482,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q39:Y39">
+  <conditionalFormatting sqref="Q42:Y42">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2457,7 +2492,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B40:B44">
+  <conditionalFormatting sqref="B43:B47">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
@@ -2471,7 +2506,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40:O44">
+  <conditionalFormatting sqref="C43:O47">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2481,7 +2516,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P40:P44">
+  <conditionalFormatting sqref="P43:P47">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2491,8 +2526,42 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q40:Y44">
+  <conditionalFormatting sqref="Q43:Y47">
     <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:B30">
+    <cfRule type="dataBar" priority="42">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{4522925B-D263-4740-830B-036B98A7E6A9}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:P8 P9:P30">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q8:Y30">
+    <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2506,17 +2575,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4522925B-D263-4740-830B-036B98A7E6A9}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>B9:B27</xm:sqref>
-        </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{AD0E4649-9E72-4706-9164-C3BAE99F2B77}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
@@ -2539,7 +2597,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>B28</xm:sqref>
+          <xm:sqref>B31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6B198507-AB3D-48F7-B35A-BB1C23ECD2AE}">
@@ -2550,7 +2608,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>B29:B33</xm:sqref>
+          <xm:sqref>B32:B36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{67B2350F-4AD0-43FF-A8C1-9834E99D7167}">
@@ -2561,7 +2619,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>B34:B38</xm:sqref>
+          <xm:sqref>B37:B41</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{75E7E111-2662-4970-8FE4-18A7021B4F10}">
@@ -2572,7 +2630,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>B39</xm:sqref>
+          <xm:sqref>B42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{5E8C772E-FC63-4698-9963-8A3BB3C13964}">
@@ -2583,7 +2641,18 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>B40:B44</xm:sqref>
+          <xm:sqref>B43:B47</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{4522925B-D263-4740-830B-036B98A7E6A9}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B9:B30</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>